<commit_message>
Updated controller mapping and a few other cosmetic changes
</commit_message>
<xml_diff>
--- a/2020CompetitionBot/Joystick Mapping 2020.xlsx
+++ b/2020CompetitionBot/Joystick Mapping 2020.xlsx
@@ -16,17 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
-  <si>
-    <t>Operator Joystick</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Kill Everything</t>
   </si>
   <si>
-    <t>Driver Joystick</t>
-  </si>
-  <si>
     <t>Up-Shift</t>
   </si>
   <si>
@@ -63,33 +57,18 @@
     <t>These are typically used for debugging or manual override</t>
   </si>
   <si>
-    <t>Intake</t>
-  </si>
-  <si>
-    <t>Climb Adjust Left</t>
-  </si>
-  <si>
     <t>Vision-Align Short</t>
   </si>
   <si>
     <t>Drive Forwards/Backwards</t>
   </si>
   <si>
-    <t>Disable Auto-Shift</t>
-  </si>
-  <si>
-    <t>Climb Adjust Right</t>
-  </si>
-  <si>
     <t>Vision-Align Long</t>
   </si>
   <si>
     <t>Turn Left/Right</t>
   </si>
   <si>
-    <t>v0.3 (Mar 1, 2020)</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -102,37 +81,61 @@
     <t>*Raise/Lower Climb</t>
   </si>
   <si>
-    <t>(Control Panel Arm Fold/Unfold)</t>
-  </si>
-  <si>
-    <t>(Vision Align and Shoot Far)</t>
-  </si>
-  <si>
-    <t>(Vision Align and Shoot Close)</t>
-  </si>
-  <si>
     <t>Control Panel Rotate 3x</t>
   </si>
   <si>
     <t>Control Panel Rotate to Colour</t>
   </si>
   <si>
-    <t>(Shoot Close)</t>
-  </si>
-  <si>
-    <t>(Shoot Far)</t>
-  </si>
-  <si>
     <t>(Control Panel Rotate)</t>
   </si>
   <si>
     <t>(Raise/Lower Hood)</t>
   </si>
   <si>
-    <t>*[Climb Arm Release with Down-Shift]</t>
-  </si>
-  <si>
-    <t>(Functionality in brackets not yet done)</t>
+    <t>Control Panel Arm Fold/Unfold</t>
+  </si>
+  <si>
+    <t>Operator Controller</t>
+  </si>
+  <si>
+    <t>Driver Controller</t>
+  </si>
+  <si>
+    <t>v0.5 (Mar 2, 2020)</t>
+  </si>
+  <si>
+    <t>Climb Arm Lock</t>
+  </si>
+  <si>
+    <t>*[see Shift table]</t>
+  </si>
+  <si>
+    <t>Expel (hold)</t>
+  </si>
+  <si>
+    <t>Intake (hold)</t>
+  </si>
+  <si>
+    <t>Shoot Far (hold)</t>
+  </si>
+  <si>
+    <t>Vision Align and Shoot Far (hold)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (hold) Vision Align and Shoot Close</t>
+  </si>
+  <si>
+    <t>(hold )Shoot Close</t>
+  </si>
+  <si>
+    <t>Disable Auto-Shift (hold)</t>
+  </si>
+  <si>
+    <t>Climb Adjust Right (hold)</t>
+  </si>
+  <si>
+    <t>(hold) Climb Adjust Left</t>
   </si>
 </sst>
 </file>
@@ -236,18 +239,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -452,12 +449,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -473,7 +464,13 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -518,7 +515,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -528,7 +525,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -567,7 +564,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -577,7 +574,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -892,7 +889,7 @@
   <dimension ref="B1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -906,20 +903,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="18.75">
-      <c r="C1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="C1" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
       <c r="H1" s="18" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="26.1" customHeight="1">
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="3"/>
@@ -931,81 +928,85 @@
     </row>
     <row r="4" spans="2:11" ht="26.1" customHeight="1">
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="H4" s="6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="K4" s="18"/>
     </row>
     <row r="5" spans="2:11" ht="26.1" customHeight="1">
       <c r="B5" s="3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="H5" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="K5" s="18"/>
     </row>
     <row r="6" spans="2:11" ht="26.1" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="H6" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K6" s="18"/>
     </row>
     <row r="7" spans="2:11" ht="26.1" customHeight="1">
       <c r="B7" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="H7" s="9"/>
+      <c r="H7" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="K7" s="18"/>
     </row>
     <row r="8" spans="2:11" ht="26.1" customHeight="1">
       <c r="B8" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="H8" s="7" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="K8" s="18"/>
     </row>
     <row r="9" spans="2:11" ht="26.1" customHeight="1">
       <c r="B9" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="H9" s="10" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="26.1" customHeight="1">
-      <c r="B10" s="4"/>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="C10" s="12"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1014,50 +1015,47 @@
       <c r="I10" s="19"/>
     </row>
     <row r="11" spans="2:11" ht="26.1" customHeight="1">
-      <c r="B11" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="C11" s="11"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="H11" s="30" t="s">
-        <v>27</v>
+      <c r="H11" s="28" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="26.1" customHeight="1">
       <c r="B12" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="H12" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:11">
       <c r="D13"/>
     </row>
     <row r="14" spans="2:11">
-      <c r="C14" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
+      <c r="C14" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
     </row>
     <row r="15" spans="2:11">
       <c r="C15" s="13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>24</v>
+        <v>10</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>17</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="15"/>
@@ -1066,31 +1064,29 @@
     </row>
     <row r="16" spans="2:11">
       <c r="C16" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="33" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>29</v>
       </c>
       <c r="F16" s="20"/>
       <c r="G16" s="22"/>
-      <c r="H16" s="35" t="s">
-        <v>38</v>
-      </c>
+      <c r="H16" s="35"/>
       <c r="I16" s="25"/>
       <c r="J16" s="25"/>
     </row>
     <row r="17" spans="2:10">
       <c r="C17" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="33" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>11</v>
       </c>
       <c r="F17" s="20"/>
       <c r="G17" s="22"/>
@@ -1099,13 +1095,13 @@
     </row>
     <row r="18" spans="2:10">
       <c r="C18" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="34" t="s">
-        <v>25</v>
+        <v>8</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>18</v>
       </c>
       <c r="F18" s="20"/>
       <c r="G18" s="22"/>
@@ -1114,13 +1110,13 @@
     </row>
     <row r="19" spans="2:10">
       <c r="C19" s="17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="33" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>11</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>
@@ -1128,13 +1124,13 @@
       <c r="J19" s="25"/>
     </row>
     <row r="21" spans="2:10" ht="18.75">
-      <c r="C21" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
+      <c r="C21" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
       <c r="H21" s="18"/>
     </row>
     <row r="23" spans="2:10" ht="26.1" customHeight="1">
@@ -1144,31 +1140,31 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="H23" s="5" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="26.1" customHeight="1">
       <c r="B24" s="4" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="H24" s="6" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="26.1" customHeight="1">
       <c r="B25" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="H25" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="26.1" customHeight="1">
@@ -1210,12 +1206,12 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="H30" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="26.1" customHeight="1">
       <c r="B31" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="3"/>
@@ -1225,14 +1221,14 @@
     </row>
     <row r="32" spans="2:10" ht="26.1" customHeight="1">
       <c r="B32" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="H32" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:8">

</xml_diff>

<commit_message>
Updated controller map and disabled colour printfs
</commit_message>
<xml_diff>
--- a/2020CompetitionBot/Joystick Mapping 2020.xlsx
+++ b/2020CompetitionBot/Joystick Mapping 2020.xlsx
@@ -27,19 +27,19 @@
     <t xml:space="preserve">Operator Joystick</t>
   </si>
   <si>
-    <t xml:space="preserve">v0.4 (Mar , 2020)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Vision Align and Shoot Close)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Vision Align and Shoot Far)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Shoot Close)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Shoot Far)</t>
+    <t xml:space="preserve">v1.0 (Mar 7, 2020)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto Shoot Close</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto Shoot Far</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shoot Close</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shoot Far</t>
   </si>
   <si>
     <t xml:space="preserve">Control Panel Rotate 3x</t>
@@ -51,13 +51,13 @@
     <t xml:space="preserve">Up-Shift</t>
   </si>
   <si>
-    <t xml:space="preserve">(Control Panel Arm Fold/Unfold)</t>
+    <t xml:space="preserve">Control Panel Arm Fold/Unfold</t>
   </si>
   <si>
     <t xml:space="preserve">Left-Shift</t>
   </si>
   <si>
-    <t xml:space="preserve">Expel</t>
+    <t xml:space="preserve">Expel (when moving forward)</t>
   </si>
   <si>
     <t xml:space="preserve">Down-Shift</t>
@@ -69,7 +69,7 @@
     <t xml:space="preserve">Right-Shift</t>
   </si>
   <si>
-    <t xml:space="preserve">*[Climb Arm Release with Down-Shift]</t>
+    <t xml:space="preserve">*[Climb Arm with Shifts]</t>
   </si>
   <si>
     <t xml:space="preserve">(Control Panel Rotate)</t>
@@ -96,13 +96,10 @@
     <t xml:space="preserve">Up</t>
   </si>
   <si>
-    <t xml:space="preserve">(Raise/Lower Hood)</t>
-  </si>
-  <si>
     <t xml:space="preserve">-</t>
   </si>
   <si>
-    <t xml:space="preserve">(Functionality in brackets not yet done)</t>
+    <t xml:space="preserve">Climb Arm Lock</t>
   </si>
   <si>
     <t xml:space="preserve">Right</t>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t xml:space="preserve">Vision-Align Long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backup 1 foot</t>
   </si>
   <si>
     <t xml:space="preserve">Turn Left/Right</t>
@@ -151,7 +151,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -199,18 +199,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFCC9900"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -275,18 +263,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -386,7 +368,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -419,24 +401,28 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -444,14 +430,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -463,10 +441,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -479,7 +453,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -495,7 +469,31 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -503,31 +501,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -535,11 +509,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -620,9 +594,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>95400</xdr:colOff>
+      <xdr:colOff>95760</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:rowOff>9720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
@@ -642,8 +616,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4368600" y="437760"/>
-          <a:ext cx="5978880" cy="3323880"/>
+          <a:off x="4369680" y="438120"/>
+          <a:ext cx="5978520" cy="3323520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -658,15 +632,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>85680</xdr:colOff>
+      <xdr:colOff>86040</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1207440</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>331200</xdr:rowOff>
+      <xdr:rowOff>330840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -680,8 +654,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4358880" y="5695920"/>
-          <a:ext cx="5978880" cy="3314160"/>
+          <a:off x="4359960" y="5680800"/>
+          <a:ext cx="5978520" cy="3313800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -704,12 +678,12 @@
   <dimension ref="B1:K35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="19.71"/>
@@ -763,7 +737,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="11" t="s">
         <v>7</v>
       </c>
       <c r="K5" s="4"/>
@@ -776,7 +750,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="12" t="s">
         <v>9</v>
       </c>
       <c r="K6" s="4"/>
@@ -789,7 +763,7 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="13" t="s">
         <v>11</v>
       </c>
       <c r="K7" s="4"/>
@@ -802,7 +776,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="14" t="s">
         <v>13</v>
       </c>
       <c r="K8" s="4"/>
@@ -815,7 +789,7 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="15" t="s">
         <v>15</v>
       </c>
     </row>
@@ -826,7 +800,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="H10" s="11"/>
-      <c r="I10" s="17"/>
+      <c r="I10" s="16"/>
     </row>
     <row r="11" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="7" t="s">
@@ -836,7 +810,7 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="17" t="s">
         <v>17</v>
       </c>
     </row>
@@ -848,100 +822,98 @@
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="22"/>
-      <c r="G15" s="24"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="26" t="s">
+      <c r="F15" s="20"/>
+      <c r="G15" s="22"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="29"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="31" t="s">
+      <c r="F16" s="27"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="26" t="s">
+      <c r="D17" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="27"/>
+      <c r="G17" s="28"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="30"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="30"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="32"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="26" t="s">
+      <c r="D18" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="E18" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="35" t="s">
+      <c r="F18" s="27"/>
+      <c r="G18" s="28"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="29"/>
-      <c r="G18" s="30"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="27"/>
-      <c r="G19" s="37"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
+      <c r="D19" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="25"/>
+      <c r="G19" s="35"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="21" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -955,32 +927,32 @@
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="H23" s="12" t="s">
-        <v>33</v>
+      <c r="H23" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
-      <c r="H24" s="19" t="s">
-        <v>35</v>
+      <c r="H24" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-      <c r="H25" s="12" t="s">
-        <v>37</v>
+      <c r="H25" s="11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -989,7 +961,7 @@
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
-      <c r="H26" s="13"/>
+      <c r="H26" s="12"/>
     </row>
     <row r="27" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="7"/>
@@ -997,7 +969,7 @@
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
-      <c r="H27" s="38"/>
+      <c r="H27" s="36"/>
     </row>
     <row r="28" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="5"/>
@@ -1005,7 +977,9 @@
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="H28" s="15"/>
+      <c r="H28" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="7"/>
@@ -1013,7 +987,7 @@
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
-      <c r="H29" s="16"/>
+      <c r="H29" s="15"/>
     </row>
     <row r="30" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="5"/>
@@ -1021,7 +995,7 @@
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
-      <c r="H30" s="19" t="s">
+      <c r="H30" s="8" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1033,7 +1007,7 @@
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
-      <c r="H31" s="18"/>
+      <c r="H31" s="17"/>
     </row>
     <row r="32" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="5" t="s">
@@ -1043,7 +1017,7 @@
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
-      <c r="H32" s="19" t="s">
+      <c r="H32" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1061,7 +1035,7 @@
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
-      <c r="H34" s="12"/>
+      <c r="H34" s="11"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="5"/>

</xml_diff>

<commit_message>
created pre spin command
</commit_message>
<xml_diff>
--- a/2020CompetitionBot/Joystick Mapping 2020.xlsx
+++ b/2020CompetitionBot/Joystick Mapping 2020.xlsx
@@ -30,7 +30,7 @@
     <t xml:space="preserve">v1.0 (Mar 7, 2020)</t>
   </si>
   <si>
-    <t xml:space="preserve">Auto Shoot Close</t>
+    <t xml:space="preserve">Spin Up Flywheel</t>
   </si>
   <si>
     <t xml:space="preserve">Auto Shoot Far</t>
@@ -600,9 +600,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1217160</xdr:colOff>
+      <xdr:colOff>1216800</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>18360</xdr:rowOff>
+      <xdr:rowOff>18000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -616,8 +616,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4369680" y="438120"/>
-          <a:ext cx="5978520" cy="3323520"/>
+          <a:off x="4370400" y="438120"/>
+          <a:ext cx="5978160" cy="3323160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -638,9 +638,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1207440</xdr:colOff>
+      <xdr:colOff>1207080</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>330840</xdr:rowOff>
+      <xdr:rowOff>330480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -654,8 +654,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4359960" y="5680800"/>
-          <a:ext cx="5978520" cy="3313800"/>
+          <a:off x="4360680" y="5680800"/>
+          <a:ext cx="5978160" cy="3313440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -678,7 +678,7 @@
   <dimension ref="B1:K35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>